<commit_message>
Se elimino el servo motor del codigo
</commit_message>
<xml_diff>
--- a/localizacion.xlsx
+++ b/localizacion.xlsx
@@ -1,38 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PORTAFOLIO DE DESAROLLO__ALEJANDRO GIRALDO OCAMPO\ARDUINO\PRACTICAS\Puerta de Seguridad\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EB1EF7-2E89-4FF9-B487-4E6A43937236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>FECHA</t>
   </si>
   <si>
     <t>LOCALIZACIÓN</t>
   </si>
+  <si>
+    <t>2022-11-11 10:18:01.798523</t>
+  </si>
+  <si>
+    <t>Calle 35, Santa Teresita, Comuna 12 - La América, Perímetro Urbano Medellín, Medellín, Valle de Aburrá, Antioquia, 050032, Colombia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,22 +68,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{34609CD1-8C0A-4C94-B498-3F6735E04E11}"/>
-  </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -125,7 +115,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -157,27 +147,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -209,24 +181,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -402,20 +356,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
-    <col min="2" max="2" width="140.5703125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -423,6 +371,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambiando Comentarios del Proyectos
</commit_message>
<xml_diff>
--- a/localizacion.xlsx
+++ b/localizacion.xlsx
@@ -22,10 +22,10 @@
     <t>LOCALIZACIÓN</t>
   </si>
   <si>
-    <t>2022-11-11 11:33:00.188160</t>
+    <t>2022-11-11 12:13:16.225915</t>
   </si>
   <si>
-    <t>Calle 35, Santa Teresita, Comuna 12 - La América, Perímetro Urbano Medellín, Medellín, Valle de Aburrá, Antioquia, 050032, Colombia</t>
+    <t>Unillaves, 34C-40, Carrera 87C, Santa Teresita, Comuna 12 - La América, Perímetro Urbano Medellín, Medellín, Valle de Aburrá, Antioquia, 050032, Colombia</t>
   </si>
 </sst>
 </file>

</xml_diff>